<commit_message>
Add additional parameters, continue to reformat sheets, improve enum parsing.
</commit_message>
<xml_diff>
--- a/Battelle.EPA.WideAreaDecon.API.Tests/InputFiles/ParameterTests/ParameterMetaDataTests.xlsx
+++ b/Battelle.EPA.WideAreaDecon.API.Tests/InputFiles/ParameterTests/ParameterMetaDataTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\EPA\WideAreaDecon\Battelle.EPA.WideAreaDecon.API.Tests\InputFiles\ParameterTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7A7945-FA34-493E-8EF9-934DE3713EB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE0E562-D1CC-489D-AECD-C011C619B737}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>Internal</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Units</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Distribution Type</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>Parameter 6</t>
   </si>
   <si>
-    <t>Parameter 7</t>
-  </si>
-  <si>
     <t>Lower Limit</t>
   </si>
   <si>
@@ -123,27 +117,12 @@
     <t>Units 4</t>
   </si>
   <si>
-    <t>Note 1</t>
-  </si>
-  <si>
-    <t>Note 2</t>
-  </si>
-  <si>
-    <t>Note 3</t>
-  </si>
-  <si>
-    <t>Note 4</t>
-  </si>
-  <si>
     <t>Test 0</t>
   </si>
   <si>
     <t>Units 0</t>
   </si>
   <si>
-    <t>Note 0</t>
-  </si>
-  <si>
     <t>Test Description 0</t>
   </si>
   <si>
@@ -162,12 +141,6 @@
     <t>Surface Type</t>
   </si>
   <si>
-    <t>Application Method</t>
-  </si>
-  <si>
-    <t>Gel</t>
-  </si>
-  <si>
     <t>HVAC</t>
   </si>
   <si>
@@ -189,19 +162,7 @@
     <t>Units 6</t>
   </si>
   <si>
-    <t>Note 5</t>
-  </si>
-  <si>
-    <t>Note 6</t>
-  </si>
-  <si>
-    <t>Physical</t>
-  </si>
-  <si>
     <t>OutdoorExterior</t>
-  </si>
-  <si>
-    <t>LiquidSpray</t>
   </si>
   <si>
     <t>Roofing</t>
@@ -528,18 +489,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="17" width="13.7109375" customWidth="1"/>
+    <col min="1" max="15" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -586,237 +547,198 @@
         <v>14</v>
       </c>
       <c r="P1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>10</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>10</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>10</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>10</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6">
+        <v>1.5</v>
+      </c>
+      <c r="N6">
+        <v>100.5</v>
+      </c>
+      <c r="O6">
+        <v>0.01</v>
+      </c>
+      <c r="P6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7">
+        <v>1.5</v>
+      </c>
+      <c r="N7">
+        <v>100.5</v>
+      </c>
+      <c r="O7">
+        <v>0.01</v>
+      </c>
+      <c r="P7" t="s">
         <v>45</v>
       </c>
-      <c r="S1" t="s">
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>10</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>10</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>10</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>10</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O6">
+      <c r="M8">
         <v>1.5</v>
       </c>
-      <c r="P6">
+      <c r="N8">
         <v>100.5</v>
       </c>
-      <c r="Q6">
+      <c r="O8">
         <v>0.01</v>
       </c>
-      <c r="R6" t="s">
+      <c r="P8" t="s">
         <v>46</v>
-      </c>
-      <c r="S6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" t="s">
-        <v>54</v>
-      </c>
-      <c r="O7">
-        <v>1.5</v>
-      </c>
-      <c r="P7">
-        <v>100.5</v>
-      </c>
-      <c r="Q7">
-        <v>0.01</v>
-      </c>
-      <c r="R7" t="s">
-        <v>56</v>
-      </c>
-      <c r="S7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" t="s">
-        <v>55</v>
-      </c>
-      <c r="O8">
-        <v>1.5</v>
-      </c>
-      <c r="P8">
-        <v>100.5</v>
-      </c>
-      <c r="Q8">
-        <v>0.01</v>
-      </c>
-      <c r="R8" t="s">
-        <v>58</v>
-      </c>
-      <c r="S8" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>